<commit_message>
varialbles with different distributions (i.e. pert, normal, uniform)
</commit_message>
<xml_diff>
--- a/examples/Reference_2_params.xlsx
+++ b/examples/Reference_2_params.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t xml:space="preserve">Classification</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t xml:space="preserve">Power block efficiency at design point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">normal</t>
   </si>
   <si>
     <t xml:space="preserve">CONTROL SYSTEM</t>
@@ -549,7 +552,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G18" activeCellId="0" sqref="G18"/>
+      <selection pane="bottomRight" activeCell="I18" activeCellId="0" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -820,14 +823,12 @@
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="H18" s="2" t="n">
         <v>0.05</v>
       </c>
-      <c r="I18" s="2" t="n">
-        <v>0.08</v>
-      </c>
+      <c r="I18" s="2"/>
       <c r="J18" s="2"/>
       <c r="K18" s="0" t="s">
         <v>20</v>
@@ -861,7 +862,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -902,7 +903,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>

</xml_diff>

<commit_message>
revised the types and boundaries
</commit_message>
<xml_diff>
--- a/examples/Reference_2_params.xlsx
+++ b/examples/Reference_2_params.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t xml:space="preserve">Classification</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t xml:space="preserve">STORAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t_storage</t>
   </si>
   <si>
     <t xml:space="preserve">POWER BLOCK</t>
@@ -552,7 +555,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I18" activeCellId="0" sqref="I18"/>
+      <selection pane="bottomRight" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -627,7 +630,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>2.5</v>
+        <v>2.4</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
@@ -637,8 +640,12 @@
         <v>2</v>
       </c>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="H5" s="2" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="I5" s="2" t="n">
+        <v>3.8</v>
+      </c>
       <c r="J5" s="2" t="s">
         <v>14</v>
       </c>
@@ -768,14 +775,24 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>11</v>
+      </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
+      <c r="H15" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>18</v>
+      </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
@@ -794,7 +811,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -810,20 +827,20 @@
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1"/>
       <c r="B18" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>0.3774</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H18" s="2" t="n">
         <v>0.05</v>
@@ -862,7 +879,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -903,7 +920,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>

</xml_diff>

<commit_message>
add 0 type parameters for demonstration
</commit_message>
<xml_diff>
--- a/examples/Reference_2_params.xlsx
+++ b/examples/Reference_2_params.xlsx
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t xml:space="preserve">Classification</t>
   </si>
@@ -125,6 +125,15 @@
     <t xml:space="preserve">assumed</t>
   </si>
   <si>
+    <t xml:space="preserve">A_heliostat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heliostat reflective area</t>
+  </si>
+  <si>
     <t xml:space="preserve">RECEIVER</t>
   </si>
   <si>
@@ -137,10 +146,19 @@
     <t xml:space="preserve">pert</t>
   </si>
   <si>
+    <t xml:space="preserve">ab_rec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Receiver coating absorptance</t>
+  </si>
+  <si>
     <t xml:space="preserve">STORAGE</t>
   </si>
   <si>
     <t xml:space="preserve">t_storage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">h</t>
   </si>
   <si>
     <t xml:space="preserve">POWER BLOCK</t>
@@ -548,14 +566,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:K30"/>
+  <dimension ref="A2:K32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I16" activeCellId="0" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="J26" activeCellId="0" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -687,23 +705,33 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>169</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>0</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="K9" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -716,52 +744,74 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="2" t="n">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="n">
         <v>0.05</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" s="2" t="n">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="H11" s="2" t="n">
+      <c r="G12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="2" t="n">
         <v>0.01</v>
       </c>
-      <c r="I11" s="2" t="n">
+      <c r="I12" s="2" t="n">
         <v>0.09</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="0" t="s">
+      <c r="J12" s="2"/>
+      <c r="K12" s="0" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -773,31 +823,11 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="I15" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-    </row>
+    <row r="15" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2"/>
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -810,49 +840,47 @@
       <c r="K16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="A17" s="1"/>
+      <c r="B17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="n">
+        <v>2</v>
+      </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
+      <c r="H17" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I17" s="2" t="n">
+        <v>18</v>
+      </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>0.3774</v>
-      </c>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" s="2" t="n">
-        <v>0.05</v>
-      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
-      <c r="K18" s="0" t="s">
-        <v>20</v>
-      </c>
+      <c r="K18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -865,22 +893,34 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
+      <c r="A20" s="1"/>
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>0.3774</v>
+      </c>
       <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="2" t="n">
+        <v>0.05</v>
+      </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
+      <c r="K20" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -906,7 +946,9 @@
       <c r="K22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2"/>
+      <c r="A23" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -919,9 +961,7 @@
       <c r="K23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>32</v>
-      </c>
+      <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -947,7 +987,9 @@
       <c r="K25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2"/>
+      <c r="A26" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1011,6 +1053,32 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
     </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="2"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
correct excel 0 type parameter updates
</commit_message>
<xml_diff>
--- a/examples/Reference_2_params.xlsx
+++ b/examples/Reference_2_params.xlsx
@@ -573,7 +573,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J26" activeCellId="0" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -898,7 +898,7 @@
         <v>34</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>0.3774</v>
+        <v>0.5</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">

</xml_diff>

<commit_message>
solved mp issue, dict Python3, pert dist
</commit_message>
<xml_diff>
--- a/examples/Reference_2_params.xlsx
+++ b/examples/Reference_2_params.xlsx
@@ -22,7 +22,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Y</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="D2" authorId="0">
@@ -492,7 +492,7 @@
     <cellStyle name="Hyperlink 9" xfId="32"/>
     <cellStyle name="Neutral 12" xfId="33"/>
     <cellStyle name="Note 7" xfId="34"/>
-    <cellStyle name="Result" xfId="35"/>
+    <cellStyle name="Result 1" xfId="35"/>
     <cellStyle name="Result2" xfId="36"/>
     <cellStyle name="Status 10" xfId="37"/>
     <cellStyle name="Text 6" xfId="38"/>
@@ -562,7 +562,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -573,15 +573,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.37"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="65.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.48"/>
@@ -589,7 +588,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="93.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="89.47"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -777,7 +775,7 @@
         <v>27</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="I12" s="2" t="n">
         <v>0.09</v>
@@ -803,7 +801,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="H13" s="2" t="n">
         <v>0.88</v>

</xml_diff>

<commit_message>
revise lhs sample to uniform dist include des params
</commit_message>
<xml_diff>
--- a/examples/Reference_2_params.xlsx
+++ b/examples/Reference_2_params.xlsx
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t xml:space="preserve">Classification</t>
   </si>
@@ -149,6 +149,9 @@
     <t xml:space="preserve">he_av_design</t>
   </si>
   <si>
+    <t xml:space="preserve">p</t>
+  </si>
+  <si>
     <t xml:space="preserve">uniform</t>
   </si>
   <si>
@@ -173,9 +176,6 @@
     <t xml:space="preserve">rec_fr</t>
   </si>
   <si>
-    <t xml:space="preserve">pert</t>
-  </si>
-  <si>
     <t xml:space="preserve">Receiver loss fraction of radiance at design point</t>
   </si>
   <si>
@@ -201,9 +201,6 @@
   </si>
   <si>
     <t xml:space="preserve">eff_blk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">normal</t>
   </si>
   <si>
     <t xml:space="preserve">Power block efficiency at design point</t>
@@ -616,10 +613,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H20" activeCellId="1" sqref="H8 H20"/>
+      <selection pane="bottomRight" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.93"/>
@@ -733,10 +730,14 @@
       <c r="E8" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>1</v>
+      </c>
       <c r="H8" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I8" s="2" t="n">
         <v>0.985</v>
@@ -745,22 +746,22 @@
         <v>0.995</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>169</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E9" s="2" t="n">
         <v>0</v>
@@ -771,10 +772,10 @@
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -793,7 +794,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -810,19 +811,19 @@
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>0.05</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="I12" s="2" t="n">
         <v>0.03</v>
@@ -834,7 +835,7 @@
         <v>27</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -849,10 +850,14 @@
       <c r="E13" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="2" t="n">
+        <v>-1</v>
+      </c>
       <c r="H13" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I13" s="2" t="n">
         <v>0.88</v>
@@ -864,7 +869,7 @@
         <v>29</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -966,22 +971,18 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" s="2" t="n">
-        <v>0.05</v>
-      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1014,7 +1015,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1058,7 +1059,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>

</xml_diff>

<commit_message>
update contingency, solstice windy, and msys action test
</commit_message>
<xml_diff>
--- a/examples/Reference_2_params.xlsx
+++ b/examples/Reference_2_params.xlsx
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t xml:space="preserve">Classification</t>
   </si>
@@ -613,10 +613,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="F29" activeCellId="0" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.93"/>
@@ -822,9 +822,7 @@
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="H12" s="2"/>
       <c r="I12" s="2" t="n">
         <v>0.03</v>
       </c>

</xml_diff>